<commit_message>
Refactoring e miglioramento gestione interops
</commit_message>
<xml_diff>
--- a/AAA Files for demo/Input files/CN43N.xlsx
+++ b/AAA Files for demo/Input files/CN43N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fperrino\Desktop\KPI UT_LAVORO_LEFO\Files\File Originali\SuperDettagli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\AAA Files for demo\Input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABF803B-1292-43FF-86F1-1D19AFEF2BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961EA45A-499B-4722-9A9D-962357738B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="24">
   <si>
     <t>Level</t>
   </si>
@@ -553,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A34" sqref="A34:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +700,1938 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="9"/>
+      <c r="M21" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="9"/>
+      <c r="M23" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="9"/>
+      <c r="M27" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="M32" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33" s="9"/>
+      <c r="M33" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N33" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="9"/>
+      <c r="M35" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="5"/>
+      <c r="M36" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="9"/>
+      <c r="M37" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="5"/>
+      <c r="M38" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L39" s="9"/>
+      <c r="M39" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N39" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="5"/>
+      <c r="M40" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" s="9"/>
+      <c r="M41" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N41" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L42" s="5"/>
+      <c r="M42" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="9"/>
+      <c r="M43" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N43" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L44" s="5"/>
+      <c r="M44" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L45" s="9"/>
+      <c r="M45" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N45" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="9"/>
+      <c r="M47" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N47" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="6">
+        <v>42369</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L48" s="5"/>
+      <c r="M48" s="6">
+        <v>42145</v>
+      </c>
+      <c r="N48" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="10">
+        <v>42369</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L49" s="9"/>
+      <c r="M49" s="10">
+        <v>42145</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>